<commit_message>
updated codebook based on our 4/5 meeting
Former-commit-id: aa9760464fbb6ef311bcaac1087b56130b463319
</commit_message>
<xml_diff>
--- a/Classifications/codebook.xlsx
+++ b/Classifications/codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/Classifications/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/krector_uiowa_edu/Documents/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{49527AEF-2174-4DEF-B178-1B2CF209FEB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DF6DC365-4653-4E66-94F9-18AACB3CF997}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{49527AEF-2174-4DEF-B178-1B2CF209FEB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{77DF8ED8-132B-4C71-917D-6705A5772E50}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{34121A93-6F05-48B3-9649-C08D748189D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{34121A93-6F05-48B3-9649-C08D748189D7}"/>
   </bookViews>
   <sheets>
     <sheet name="body-based helpful" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>squats, jumping jacks</t>
   </si>
   <si>
-    <t>Which limb to move</t>
-  </si>
-  <si>
     <t>Specifies what body part to move</t>
   </si>
   <si>
@@ -200,7 +197,7 @@
     <t>5 4 3 2 1, down down, up up, in in, hop hop</t>
   </si>
   <si>
-    <t>CONCERN</t>
+    <t>Body Parts</t>
   </si>
 </sst>
 </file>
@@ -561,21 +558,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6466B393-F1B8-46F8-A991-A3DF9DAFECE3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,11 +582,9 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -600,37 +595,48 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -643,17 +649,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -672,10 +678,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -683,21 +689,21 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -705,10 +711,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -716,18 +722,18 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -738,20 +744,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF67C7AC-66B8-4B1E-9499-3043B122A578}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,81 +768,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated codebook based on domain stakeholder feedback
Former-commit-id: 90c056e0f30f09781640b707f3727b55e2aa6fb2
</commit_message>
<xml_diff>
--- a/Classifications/codebook.xlsx
+++ b/Classifications/codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/krector_uiowa_edu/Documents/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{49527AEF-2174-4DEF-B178-1B2CF209FEB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C20AB28B-7D15-4840-B2D3-B56099205F68}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{49527AEF-2174-4DEF-B178-1B2CF209FEB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4100CD33-6F67-4137-A492-97303E051875}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{34121A93-6F05-48B3-9649-C08D748189D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{34121A93-6F05-48B3-9649-C08D748189D7}"/>
   </bookViews>
   <sheets>
     <sheet name="body-based helpful" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>you should feel a stretch in your leg</t>
   </si>
   <si>
-    <t>Breathe</t>
-  </si>
-  <si>
     <t>Instructor reminding the person to breathe</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>Transitioning the person within or between an exercise - does not have to specify what exercise it is</t>
   </si>
   <si>
-    <t>finishing strong</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -198,13 +192,28 @@
   </si>
   <si>
     <t>Intros, Instructor and "participants" speaking with one another; if you remove it, it doesn't affect anything</t>
+  </si>
+  <si>
+    <t>Acceptable because they specify what to do with your body</t>
+  </si>
+  <si>
+    <t>Acceptable because they specify when to do the exercise</t>
+  </si>
+  <si>
+    <t>it’s over, yes all right we are done with those, we are done</t>
+  </si>
+  <si>
+    <t>Unacceptable because text does not specify what to do with body or time – with Breathing being the notable exception</t>
+  </si>
+  <si>
+    <t>Breathing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +225,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF2F5496"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,9 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6466B393-F1B8-46F8-A991-A3DF9DAFECE3}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,84 +598,90 @@
     <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A88CC-C467-4A60-B9B7-6CA6779139C4}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,67 +691,61 @@
     <col min="3" max="3" width="54.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -727,13 +753,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -744,9 +781,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF67C7AC-66B8-4B1E-9499-3043B122A578}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -757,81 +794,86 @@
     <col min="3" max="3" width="39.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated codebook based on meeting
Former-commit-id: 342f09c4f1fac2958ab4cf31745c295d3d31f806
</commit_message>
<xml_diff>
--- a/Classifications/codebook.xlsx
+++ b/Classifications/codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/krector_uiowa_edu/Documents/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{49527AEF-2174-4DEF-B178-1B2CF209FEB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4100CD33-6F67-4137-A492-97303E051875}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{49527AEF-2174-4DEF-B178-1B2CF209FEB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FD2B9005-B95A-4E8A-B49C-098A01A88154}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{34121A93-6F05-48B3-9649-C08D748189D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{34121A93-6F05-48B3-9649-C08D748189D7}"/>
   </bookViews>
   <sheets>
     <sheet name="body-based helpful" sheetId="1" r:id="rId1"/>
@@ -146,15 +146,6 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Telling a person how much time is left in an exercise</t>
-  </si>
-  <si>
-    <t>so we have 10 seconds left</t>
-  </si>
-  <si>
-    <t>getting ready, starting</t>
-  </si>
-  <si>
     <t>Now, next, repeat, another, it's going to be; just listen to my cue</t>
   </si>
   <si>
@@ -207,6 +198,15 @@
   </si>
   <si>
     <t>Breathing</t>
+  </si>
+  <si>
+    <t>Telling a person how much time is left in an exercise or a break</t>
+  </si>
+  <si>
+    <t>so we have 10 seconds left, 5 more seconds; getting ready to go</t>
+  </si>
+  <si>
+    <t>starting, let's go</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,7 +600,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -628,7 +628,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -645,7 +645,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,13 +661,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A88CC-C467-4A60-B9B7-6CA6779139C4}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,7 +693,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -715,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -734,10 +734,10 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -748,7 +748,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -759,7 +759,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -770,7 +770,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF67C7AC-66B8-4B1E-9499-3043B122A578}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,7 +796,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -812,7 +812,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>